<commit_message>
L.Regression with one model
</commit_message>
<xml_diff>
--- a/parametros_cineticos.xlsx
+++ b/parametros_cineticos.xlsx
@@ -458,481 +458,481 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>CR0 (Zero Order) Subgroup 1</t>
+          <t>CR0 Subgroup 1</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>25099.22826185446</v>
+        <v>2633.265520811323</v>
       </c>
       <c r="C2" t="n">
-        <v>33.25412749333375</v>
+        <v>0.0007202279044656574</v>
       </c>
       <c r="D2" t="n">
-        <v>0.7123225100308961</v>
+        <v>0.05450764348867843</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>CR1 (First Order) Subgroup 1</t>
+          <t>CR1 Subgroup 1</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>25288.93998012604</v>
+        <v>2741.885299681539</v>
       </c>
       <c r="C3" t="n">
-        <v>36.16260746355206</v>
+        <v>0.0007906561501348794</v>
       </c>
       <c r="D3" t="n">
-        <v>0.7152791740715663</v>
+        <v>0.05825222639085226</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>CR2 (Second Order) Subgroup 1</t>
+          <t>CR2 Subgroup 1</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>25576.49002836243</v>
+        <v>2907.059354896189</v>
       </c>
       <c r="C4" t="n">
-        <v>123.1719350584639</v>
+        <v>0.002725059735176096</v>
       </c>
       <c r="D4" t="n">
-        <v>0.7196888750619088</v>
+        <v>0.064063329474777</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>CR3 (Third Order) Subgroup 1</t>
+          <t>CR3 Subgroup 1</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>25673.13525766615</v>
+        <v>2962.715762636106</v>
       </c>
       <c r="C5" t="n">
-        <v>42.84529714557096</v>
+        <v>0.0009510932762169244</v>
       </c>
       <c r="D5" t="n">
-        <v>0.7211517603266062</v>
+        <v>0.06605056052768943</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>DM1 (Parabolic law) Subgroup 1</t>
+          <t>DM1 Subgroup 1</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>56261.25662210917</v>
+        <v>11991.56429097778</v>
       </c>
       <c r="C6" t="n">
-        <v>27500.90282241346</v>
+        <v>0.001855050517804356</v>
       </c>
       <c r="D6" t="n">
-        <v>0.7606511028843865</v>
+        <v>0.2356483625798341</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>DM2 (Valensi - 2D diffusion) Subgroup 1</t>
+          <t>DM2 Subgroup 1</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>56387.20199826936</v>
+        <v>12063.57947437494</v>
       </c>
       <c r="C7" t="n">
-        <v>14497.54635442054</v>
+        <v>0.0009664084098867688</v>
       </c>
       <c r="D7" t="n">
-        <v>0.7614290076458149</v>
+        <v>0.2371782519274735</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>DM3 (Ginstling - Broushtein) Subgroup 1</t>
+          <t>DM3 Subgroup 1</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>56429.41837183055</v>
+        <v>12087.76090545364</v>
       </c>
       <c r="C8" t="n">
-        <v>3279.307837194239</v>
+        <v>0.0002177353319765159</v>
       </c>
       <c r="D8" t="n">
-        <v>0.7616893361692973</v>
+        <v>0.237691382819225</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>NG1.5 (Avrami - Erofeev - n = 1.5) Subgroup 1</t>
+          <t>NG1.5 Subgroup 1</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>14838.35995395058</v>
+        <v>-413.7542166640237</v>
       </c>
       <c r="C9" t="n">
-        <v>2.884139493848685</v>
+        <v>-0.0001417506002811621</v>
       </c>
       <c r="D9" t="n">
-        <v>0.6557558814086574</v>
+        <v>0.003063051899264035</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>NG2 (Avrami - Erofeev - n = 2) Subgroup 1</t>
+          <t>NG2 Subgroup 1</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>9613.069940862861</v>
+        <v>-1991.573974836802</v>
       </c>
       <c r="C10" t="n">
-        <v>0.6888792215538997</v>
+        <v>-0.0007437054569524939</v>
       </c>
       <c r="D10" t="n">
-        <v>0.5818661454525669</v>
+        <v>0.1092794004752168</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>NG3 (Avrami - Erofeev - n = 3) Subgroup 1</t>
+          <t>NG3 Subgroup 1</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>4387.779927775146</v>
+        <v>-3569.393733009581</v>
       </c>
       <c r="C11" t="n">
-        <v>0.1159248237915639</v>
+        <v>-0.0014528508583018</v>
       </c>
       <c r="D11" t="n">
-        <v>0.3848363154120141</v>
+        <v>0.4545533609356666</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>CR0 (Zero Order) Subgroup 2</t>
+          <t>CR0 Subgroup 2</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>33864.69060527653</v>
+        <v>88862.50469132305</v>
       </c>
       <c r="C12" t="n">
-        <v>55.68197749926017</v>
+        <v>3272643.68897705</v>
       </c>
       <c r="D12" t="n">
-        <v>0.5960600557798178</v>
+        <v>0.878690686980199</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>CR1 (First Order) Subgroup 2</t>
+          <t>CR1 Subgroup 2</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>42130.1162560579</v>
+        <v>117187.7235918807</v>
       </c>
       <c r="C13" t="n">
-        <v>473.4303693994436</v>
+        <v>2007404786.309897</v>
       </c>
       <c r="D13" t="n">
-        <v>0.5924259790729864</v>
+        <v>0.911050929229521</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>CR2 (Second Order) Subgroup 2</t>
+          <t>CR2 Subgroup 2</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>58822.75988860156</v>
+        <v>176932.3201075681</v>
       </c>
       <c r="C14" t="n">
-        <v>94571.25318916698</v>
+        <v>3678255467297659</v>
       </c>
       <c r="D14" t="n">
-        <v>0.5757746746679275</v>
+        <v>0.9373314311454858</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>CR3 (Third Order) Subgroup 2</t>
+          <t>CR3 Subgroup 2</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>65383.0787421971</v>
+        <v>200808.2932331476</v>
       </c>
       <c r="C15" t="n">
-        <v>159579.1277687355</v>
+        <v>2.405944609686192e+17</v>
       </c>
       <c r="D15" t="n">
-        <v>0.5690253497775437</v>
+        <v>0.9408074290888392</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>DM1 (Parabolic law) Subgroup 2</t>
+          <t>DM1 Subgroup 2</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>77077.55225579807</v>
+        <v>187554.2156777986</v>
       </c>
       <c r="C16" t="n">
-        <v>136199.0601310837</v>
+        <v>1094853906542244</v>
       </c>
       <c r="D16" t="n">
-        <v>0.6534062222911823</v>
+        <v>0.8901548007476798</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>DM2 (Valensi - 2D diffusion) Subgroup 2</t>
+          <t>DM2 Subgroup 2</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>81877.37819502005</v>
+        <v>203593.8047787519</v>
       </c>
       <c r="C17" t="n">
-        <v>221459.4418843865</v>
+        <v>1.939463884161662e+16</v>
       </c>
       <c r="D17" t="n">
-        <v>0.6496577627513316</v>
+        <v>0.8993983196477597</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>DM3 (Ginstling - Broushtein) Subgroup 2</t>
+          <t>DM3 Subgroup 2</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>83765.28588399298</v>
+        <v>210086.8295971398</v>
       </c>
       <c r="C18" t="n">
-        <v>78082.73894442253</v>
+        <v>1.817226349239238e+16</v>
       </c>
       <c r="D18" t="n">
-        <v>0.6480665580510617</v>
+        <v>0.903029870512559</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>NG1.5 (Avrami - Erofeev - n = 1.5) Subgroup 2</t>
+          <t>NG1.5 Subgroup 2</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>24970.68715562359</v>
+        <v>74848.74696286963</v>
       </c>
       <c r="C19" t="n">
-        <v>14.43563051723929</v>
+        <v>305771.3289966384</v>
       </c>
       <c r="D19" t="n">
-        <v>0.5374208279232522</v>
+        <v>0.9035493940430257</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>NG2 (Avrami - Erofeev - n = 2) Subgroup 2</t>
+          <t>NG2 Subgroup 2</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>16390.97260540644</v>
+        <v>53679.25864836411</v>
       </c>
       <c r="C20" t="n">
-        <v>2.149220095162553</v>
+        <v>3386.4793407898</v>
       </c>
       <c r="D20" t="n">
-        <v>0.4736702463023593</v>
+        <v>0.8951279902880382</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>NG3 (Avrami - Erofeev - n = 3) Subgroup 2</t>
+          <t>NG3 Subgroup 2</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>7811.258055189281</v>
+        <v>32509.77033385858</v>
       </c>
       <c r="C21" t="n">
-        <v>0.2323100817970628</v>
+        <v>31.6727313701562</v>
       </c>
       <c r="D21" t="n">
-        <v>0.3198917033403048</v>
+        <v>0.8749082534798314</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>CR0 (Zero Order) Subgroup 3</t>
+          <t>CR0 Subgroup 3</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>-11927.72135096844</v>
+        <v>-12038.50675612018</v>
       </c>
       <c r="C22" t="n">
-        <v>-0.01015360332113232</v>
+        <v>-0.001702427197863892</v>
       </c>
       <c r="D22" t="n">
-        <v>0.9668232256370274</v>
+        <v>0.9617670625144055</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>CR1 (First Order) Subgroup 3</t>
+          <t>CR1 Subgroup 3</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>14847.17103837766</v>
+        <v>10260.55743790905</v>
       </c>
       <c r="C23" t="n">
-        <v>2.488256051287793</v>
+        <v>0.1886857571386683</v>
       </c>
       <c r="D23" t="n">
-        <v>0.7327218396641231</v>
+        <v>0.4708667833885153</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>CR2 (Second Order) Subgroup 3</t>
+          <t>CR2 Subgroup 3</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>197768.805885376</v>
+        <v>165147.7161863035</v>
       </c>
       <c r="C24" t="n">
-        <v>5939943613005328</v>
+        <v>48143306173680.88</v>
       </c>
       <c r="D24" t="n">
-        <v>0.9025489566290636</v>
+        <v>0.8597812835487186</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>CR3 (Third Order) Subgroup 3</t>
+          <t>CR3 Subgroup 3</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>267653.8939066047</v>
+        <v>224194.7135616544</v>
       </c>
       <c r="C25" t="n">
-        <v>5.219543788367008e+20</v>
+        <v>1.646747813823699e+18</v>
       </c>
       <c r="D25" t="n">
-        <v>0.9048715345682002</v>
+        <v>0.8649734851539975</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>DM1 (Parabolic law) Subgroup 3</t>
+          <t>DM1 Subgroup 3</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>-9240.94604470601</v>
+        <v>-9839.754331927435</v>
       </c>
       <c r="C26" t="n">
-        <v>-0.01084170878280716</v>
+        <v>-0.001822410866417914</v>
       </c>
       <c r="D26" t="n">
-        <v>0.8783705558709856</v>
+        <v>0.8721347581126049</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>DM2 (Valensi - 2D diffusion) Subgroup 3</t>
+          <t>DM2 Subgroup 3</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>-4939.59567721945</v>
+        <v>-6342.693906997762</v>
       </c>
       <c r="C27" t="n">
-        <v>-0.009624623817836808</v>
+        <v>-0.001797204070015411</v>
       </c>
       <c r="D27" t="n">
-        <v>0.4919640420774515</v>
+        <v>0.5582135757219189</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>DM3 (Ginstling - Broushtein) Subgroup 3</t>
+          <t>DM3 Subgroup 3</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>-954.808493412801</v>
+        <v>-3082.706273283913</v>
       </c>
       <c r="C28" t="n">
-        <v>-0.0009817541488496694</v>
+        <v>-0.0004292508214496291</v>
       </c>
       <c r="D28" t="n">
-        <v>0.0233229703557486</v>
+        <v>0.1575914668306114</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>NG1.5 (Avrami - Erofeev - n = 1.5) Subgroup 3</t>
+          <t>NG1.5 Subgroup 3</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>5026.615139841478</v>
+        <v>2094.61856516839</v>
       </c>
       <c r="C29" t="n">
-        <v>0.1301241514936113</v>
+        <v>0.006949074947127502</v>
       </c>
       <c r="D29" t="n">
-        <v>0.4021928224222019</v>
+        <v>0.07190325599109482</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>NG2 (Avrami - Erofeev - n = 2) Subgroup 3</t>
+          <t>NG2 Subgroup 3</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>116.3371905733864</v>
+        <v>-1988.350871201937</v>
       </c>
       <c r="C30" t="n">
-        <v>0.001183630933320994</v>
+        <v>-0.002801831497230764</v>
       </c>
       <c r="D30" t="n">
-        <v>0.0006072054191880172</v>
+        <v>0.1034152682097278</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>NG3 (Avrami - Erofeev - n = 3) Subgroup 3</t>
+          <t>NG3 Subgroup 3</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>-4793.940758694706</v>
+        <v>-6071.320307572264</v>
       </c>
       <c r="C31" t="n">
-        <v>-0.0191692824640972</v>
+        <v>-0.003633783738632058</v>
       </c>
       <c r="D31" t="n">
-        <v>0.6744246214982996</v>
+        <v>0.6771229474814363</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Code restructuring and optimization
</commit_message>
<xml_diff>
--- a/parametros_cineticos.xlsx
+++ b/parametros_cineticos.xlsx
@@ -462,13 +462,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2633.265520811323</v>
+        <v>23288.47245586674</v>
       </c>
       <c r="C2" t="n">
-        <v>0.0007202279044656574</v>
+        <v>38.15225880359203</v>
       </c>
       <c r="D2" t="n">
-        <v>0.05450764348867843</v>
+        <v>0.6628867188133686</v>
       </c>
     </row>
     <row r="3">
@@ -478,13 +478,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2741.885299681539</v>
+        <v>23884.15661053462</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0007906561501348794</v>
+        <v>49.29702604143551</v>
       </c>
       <c r="D3" t="n">
-        <v>0.05825222639085226</v>
+        <v>0.6733790583472918</v>
       </c>
     </row>
     <row r="4">
@@ -494,13 +494,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2907.059354896189</v>
+        <v>24806.89636359204</v>
       </c>
       <c r="C4" t="n">
-        <v>0.002725059735176096</v>
+        <v>219.6108457979281</v>
       </c>
       <c r="D4" t="n">
-        <v>0.064063329474777</v>
+        <v>0.6888162620334709</v>
       </c>
     </row>
     <row r="5">
@@ -510,61 +510,61 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2962.715762636106</v>
+        <v>25122.2562531207</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0009510932762169244</v>
+        <v>83.75949344712977</v>
       </c>
       <c r="D5" t="n">
-        <v>0.06605056052768943</v>
+        <v>0.6938726693684723</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>DM1 Subgroup 1</t>
+          <t>DM0 Subgroup 1</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>11991.56429097778</v>
+        <v>52896.85629800297</v>
       </c>
       <c r="C6" t="n">
-        <v>0.001855050517804356</v>
+        <v>42944.76085826926</v>
       </c>
       <c r="D6" t="n">
-        <v>0.2356483625798341</v>
+        <v>0.7213184675172366</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>DM2 Subgroup 1</t>
+          <t>DM1 Subgroup 1</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>12063.57947437494</v>
+        <v>53288.81922628694</v>
       </c>
       <c r="C7" t="n">
-        <v>0.0009664084098867688</v>
+        <v>25184.58254266901</v>
       </c>
       <c r="D7" t="n">
-        <v>0.2371782519274735</v>
+        <v>0.7240632928562425</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>DM3 Subgroup 1</t>
+          <t>DM2 Subgroup 1</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>12087.76090545364</v>
+        <v>53421.74929117745</v>
       </c>
       <c r="C8" t="n">
-        <v>0.0002177353319765159</v>
+        <v>5907.321406219426</v>
       </c>
       <c r="D8" t="n">
-        <v>0.237691382819225</v>
+        <v>0.7249887953683581</v>
       </c>
     </row>
     <row r="9">
@@ -574,13 +574,13 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-413.7542166640237</v>
+        <v>13816.13394493324</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.0001417506002811621</v>
+        <v>3.336464188559541</v>
       </c>
       <c r="D9" t="n">
-        <v>0.003063051899264035</v>
+        <v>0.6033474095103875</v>
       </c>
     </row>
     <row r="10">
@@ -590,13 +590,13 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-1991.573974836802</v>
+        <v>8782.122612132569</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.0007437054569524939</v>
+        <v>0.7254274587959104</v>
       </c>
       <c r="D10" t="n">
-        <v>0.1092794004752168</v>
+        <v>0.5171030014022349</v>
       </c>
     </row>
     <row r="11">
@@ -606,13 +606,13 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-3569.393733009581</v>
+        <v>3748.111279331875</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.0014528508583018</v>
+        <v>0.1059013586650847</v>
       </c>
       <c r="D11" t="n">
-        <v>0.4545533609356666</v>
+        <v>0.2966265781769539</v>
       </c>
     </row>
     <row r="12">
@@ -622,13 +622,13 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>88862.50469132305</v>
+        <v>40684.3195025943</v>
       </c>
       <c r="C12" t="n">
-        <v>3272643.68897705</v>
+        <v>1011.027947386652</v>
       </c>
       <c r="D12" t="n">
-        <v>0.878690686980199</v>
+        <v>0.7680722285861548</v>
       </c>
     </row>
     <row r="13">
@@ -638,13 +638,13 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>117187.7235918807</v>
+        <v>59831.05914957315</v>
       </c>
       <c r="C13" t="n">
-        <v>2007404786.309897</v>
+        <v>133335.6317832718</v>
       </c>
       <c r="D13" t="n">
-        <v>0.911050929229521</v>
+        <v>0.7591197454263598</v>
       </c>
     </row>
     <row r="14">
@@ -654,13 +654,13 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>176932.3201075681</v>
+        <v>101861.6058959529</v>
       </c>
       <c r="C14" t="n">
-        <v>3678255467297659</v>
+        <v>12422429266.50984</v>
       </c>
       <c r="D14" t="n">
-        <v>0.9373314311454858</v>
+        <v>0.7426269218723918</v>
       </c>
     </row>
     <row r="15">
@@ -670,61 +670,61 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>200808.2932331476</v>
+        <v>118831.566280088</v>
       </c>
       <c r="C15" t="n">
-        <v>2.405944609686192e+17</v>
+        <v>251607322218.1647</v>
       </c>
       <c r="D15" t="n">
-        <v>0.9408074290888392</v>
+        <v>0.7378618649909811</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>DM1 Subgroup 2</t>
+          <t>DM0 Subgroup 2</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>187554.2156777986</v>
+        <v>90513.93200219698</v>
       </c>
       <c r="C16" t="n">
-        <v>1094853906542244</v>
+        <v>34763481.07742978</v>
       </c>
       <c r="D16" t="n">
-        <v>0.8901548007476798</v>
+        <v>0.8025489485682615</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>DM2 Subgroup 2</t>
+          <t>DM1 Subgroup 2</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>203593.8047787519</v>
+        <v>101105.4581692971</v>
       </c>
       <c r="C17" t="n">
-        <v>1.939463884161662e+16</v>
+        <v>235743195.4797715</v>
       </c>
       <c r="D17" t="n">
-        <v>0.8993983196477597</v>
+        <v>0.7969355593891125</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>DM3 Subgroup 2</t>
+          <t>DM2 Subgroup 2</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>210086.8295971398</v>
+        <v>105500.7629378873</v>
       </c>
       <c r="C18" t="n">
-        <v>1.817226349239238e+16</v>
+        <v>153363870.480932</v>
       </c>
       <c r="D18" t="n">
-        <v>0.903029870512559</v>
+        <v>0.7946502055563922</v>
       </c>
     </row>
     <row r="19">
@@ -734,13 +734,13 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>74848.74696286963</v>
+        <v>36838.94176737932</v>
       </c>
       <c r="C19" t="n">
-        <v>305771.3289966384</v>
+        <v>736.3341818296014</v>
       </c>
       <c r="D19" t="n">
-        <v>0.9035493940430257</v>
+        <v>0.7299976022606572</v>
       </c>
     </row>
     <row r="20">
@@ -750,13 +750,13 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>53679.25864836411</v>
+        <v>25342.88307628239</v>
       </c>
       <c r="C20" t="n">
-        <v>3386.4793407898</v>
+        <v>47.97312139119081</v>
       </c>
       <c r="D20" t="n">
-        <v>0.8951279902880382</v>
+        <v>0.6958521485694259</v>
       </c>
     </row>
     <row r="21">
@@ -766,13 +766,13 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>32509.77033385858</v>
+        <v>13846.82438518547</v>
       </c>
       <c r="C21" t="n">
-        <v>31.6727313701562</v>
+        <v>2.482368678697976</v>
       </c>
       <c r="D21" t="n">
-        <v>0.8749082534798314</v>
+        <v>0.6085472195774219</v>
       </c>
     </row>
     <row r="22">
@@ -782,13 +782,13 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>-12038.50675612018</v>
+        <v>-12505.63654077432</v>
       </c>
       <c r="C22" t="n">
-        <v>-0.001702427197863892</v>
+        <v>-0.009898504804345587</v>
       </c>
       <c r="D22" t="n">
-        <v>0.9617670625144055</v>
+        <v>0.9836595281802547</v>
       </c>
     </row>
     <row r="23">
@@ -798,13 +798,13 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>10260.55743790905</v>
+        <v>-1836.207952824492</v>
       </c>
       <c r="C23" t="n">
-        <v>0.1886857571386683</v>
+        <v>-0.02513565892787702</v>
       </c>
       <c r="D23" t="n">
-        <v>0.4708667833885153</v>
+        <v>0.4239329919827076</v>
       </c>
     </row>
     <row r="24">
@@ -814,13 +814,13 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>165147.7161863035</v>
+        <v>53508.52173692486</v>
       </c>
       <c r="C24" t="n">
-        <v>48143306173680.88</v>
+        <v>327525.1083798885</v>
       </c>
       <c r="D24" t="n">
-        <v>0.8597812835487186</v>
+        <v>0.8161620435453979</v>
       </c>
     </row>
     <row r="25">
@@ -830,61 +830,61 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>224194.7135616544</v>
+        <v>75525.16978479302</v>
       </c>
       <c r="C25" t="n">
-        <v>1.646747813823699e+18</v>
+        <v>18122315.57321637</v>
       </c>
       <c r="D25" t="n">
-        <v>0.8649734851539975</v>
+        <v>0.8298872666862956</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>DM1 Subgroup 3</t>
+          <t>DM0 Subgroup 3</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>-9839.754331927435</v>
+        <v>-11064.9001588159</v>
       </c>
       <c r="C26" t="n">
-        <v>-0.001822410866417914</v>
+        <v>-0.01032559696440099</v>
       </c>
       <c r="D26" t="n">
-        <v>0.8721347581126049</v>
+        <v>0.9657462999810005</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>DM2 Subgroup 3</t>
+          <t>DM1 Subgroup 3</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>-6342.693906997762</v>
+        <v>-8676.21211520137</v>
       </c>
       <c r="C27" t="n">
-        <v>-0.001797204070015411</v>
+        <v>-0.010403347419393</v>
       </c>
       <c r="D27" t="n">
-        <v>0.5582135757219189</v>
+        <v>0.9264840029489525</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>DM3 Subgroup 3</t>
+          <t>DM2 Subgroup 3</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>-3082.706273283913</v>
+        <v>-6659.121455476631</v>
       </c>
       <c r="C28" t="n">
-        <v>-0.0004292508214496291</v>
+        <v>-0.003172198020610486</v>
       </c>
       <c r="D28" t="n">
-        <v>0.1575914668306114</v>
+        <v>0.8799100174518362</v>
       </c>
     </row>
     <row r="29">
@@ -894,13 +894,13 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>2094.61856516839</v>
+        <v>-5872.929609460573</v>
       </c>
       <c r="C29" t="n">
-        <v>0.006949074947127502</v>
+        <v>-0.02942752314748293</v>
       </c>
       <c r="D29" t="n">
-        <v>0.07190325599109482</v>
+        <v>0.9364025311519699</v>
       </c>
     </row>
     <row r="30">
@@ -910,13 +910,13 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>-1988.350871201937</v>
+        <v>-7891.290437778617</v>
       </c>
       <c r="C30" t="n">
-        <v>-0.002801831497230764</v>
+        <v>-0.02392281016829638</v>
       </c>
       <c r="D30" t="n">
-        <v>0.1034152682097278</v>
+        <v>0.9741242506812711</v>
       </c>
     </row>
     <row r="31">
@@ -926,13 +926,13 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>-6071.320307572264</v>
+        <v>-9909.651266096656</v>
       </c>
       <c r="C31" t="n">
-        <v>-0.003633783738632058</v>
+        <v>-0.01817555953426603</v>
       </c>
       <c r="D31" t="n">
-        <v>0.6771229474814363</v>
+        <v>0.9873993064886006</v>
       </c>
     </row>
   </sheetData>

</xml_diff>